<commit_message>
Elimino relación 'has' en el .xlsx
</commit_message>
<xml_diff>
--- a/myInstagram.xlsx
+++ b/myInstagram.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisb\Desktop\myinstagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A69E98-B7F2-4512-BD66-A13CE67FF2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10B1F7C-B7EA-491E-B2AD-B3CF6254A4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="62">
   <si>
     <t>Nombre</t>
   </si>
@@ -199,43 +199,10 @@
     <t>jin</t>
   </si>
   <si>
-    <t>USUARIO has SEGUIDOR</t>
-  </si>
-  <si>
     <t>ID_SEGUIDOR</t>
   </si>
   <si>
     <t>ID_SEGUIDO</t>
-  </si>
-  <si>
-    <t>ID_USUARIO (FK)</t>
-  </si>
-  <si>
-    <t>ID_SEGUIDOR (FK)</t>
-  </si>
-  <si>
-    <t>USUARIO has SEGUIDO</t>
-  </si>
-  <si>
-    <t>ID_UHSR (PK)</t>
-  </si>
-  <si>
-    <t>ID_UHSO (PK)</t>
-  </si>
-  <si>
-    <t>ID_SEGUIDO (FK)</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>USUARIO has FOTO</t>
-  </si>
-  <si>
-    <t>ID_UHF (PK)</t>
-  </si>
-  <si>
-    <t>ID_FOTO (FK)</t>
   </si>
   <si>
     <t xml:space="preserve">NULL </t>
@@ -285,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,18 +263,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB6D7A8"/>
         <bgColor rgb="FFB6D7A8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -342,31 +297,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,8 +542,8 @@
   </sheetPr>
   <dimension ref="A2:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -610,11 +565,11 @@
     <col min="17" max="17" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:20" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:20" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:20" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:20" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -658,11 +613,9 @@
       <c r="P6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -690,33 +643,27 @@
       <c r="I7" s="2">
         <v>5526487953</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="10">
         <v>1</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="10">
         <v>5526487953</v>
       </c>
-      <c r="P7" s="18">
-        <v>2</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="S7" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="T7" s="13" t="s">
-        <v>63</v>
-      </c>
+      <c r="P7" s="10">
+        <v>2</v>
+      </c>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -747,30 +694,24 @@
       <c r="K8" s="7">
         <v>2</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="18" t="s">
+      <c r="N8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="10">
         <v>5548731648</v>
       </c>
-      <c r="P8" s="18">
-        <v>3</v>
-      </c>
-      <c r="R8" s="14">
-        <v>1</v>
-      </c>
-      <c r="S8" s="15">
-        <v>1</v>
-      </c>
-      <c r="T8" s="15">
-        <v>1</v>
-      </c>
+      <c r="P8" s="10">
+        <v>3</v>
+      </c>
+      <c r="R8" s="12"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -801,30 +742,24 @@
       <c r="K9" s="7">
         <v>3</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="10">
         <v>5545879996</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="10">
         <v>1</v>
       </c>
-      <c r="R9" s="14">
-        <v>2</v>
-      </c>
-      <c r="S9" s="15">
-        <v>1</v>
-      </c>
-      <c r="T9" s="16">
-        <v>2</v>
-      </c>
+      <c r="R9" s="12"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="14"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -855,41 +790,29 @@
       <c r="K10" s="7">
         <v>4</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="10">
         <v>5578963452</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="10">
         <v>5</v>
       </c>
-      <c r="R10" s="14">
-        <v>3</v>
-      </c>
-      <c r="S10" s="16">
-        <v>2</v>
-      </c>
-      <c r="T10" s="16">
-        <v>3</v>
-      </c>
+      <c r="R10" s="12"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R11" s="14">
-        <v>4</v>
-      </c>
-      <c r="S11" s="16">
-        <v>2</v>
-      </c>
-      <c r="T11" s="16">
-        <v>4</v>
-      </c>
+      <c r="R11" s="12"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -920,23 +843,17 @@
         <v>5</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="14">
-        <v>5</v>
-      </c>
-      <c r="S12" s="16">
-        <v>2</v>
-      </c>
-      <c r="T12" s="16">
-        <v>5</v>
-      </c>
+      <c r="R12" s="12"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -972,18 +889,12 @@
       <c r="L13" s="5">
         <v>1</v>
       </c>
-      <c r="M13" s="18" t="s">
+      <c r="M13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R13" s="14">
-        <v>6</v>
-      </c>
-      <c r="S13" s="16">
-        <v>3</v>
-      </c>
-      <c r="T13" s="16">
-        <v>6</v>
-      </c>
+      <c r="R13" s="12"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1019,18 +930,12 @@
       <c r="L14" s="5">
         <v>1</v>
       </c>
-      <c r="M14" s="18" t="s">
+      <c r="M14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R14" s="14">
-        <v>7</v>
-      </c>
-      <c r="S14" s="16">
-        <v>3</v>
-      </c>
-      <c r="T14" s="16">
-        <v>7</v>
-      </c>
+      <c r="R14" s="12"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1066,18 +971,12 @@
       <c r="L15" s="5">
         <v>2</v>
       </c>
-      <c r="M15" s="18" t="s">
+      <c r="M15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="R15" s="14">
-        <v>8</v>
-      </c>
-      <c r="S15" s="16">
-        <v>4</v>
-      </c>
-      <c r="T15" s="16">
-        <v>8</v>
-      </c>
+      <c r="R15" s="12"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1113,11 +1012,12 @@
       <c r="L16" s="5">
         <v>2</v>
       </c>
-      <c r="M16" s="18" t="s">
+      <c r="M16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1153,14 +1053,12 @@
       <c r="L17" s="5">
         <v>2</v>
       </c>
-      <c r="M17" s="18" t="s">
+      <c r="M17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="R17" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1196,18 +1094,12 @@
       <c r="L18" s="5">
         <v>3</v>
       </c>
-      <c r="M18" s="18" t="s">
+      <c r="M18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R18" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="S18" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="T18" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="R18" s="12"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -1243,18 +1135,12 @@
       <c r="L19" s="5">
         <v>3</v>
       </c>
-      <c r="M19" s="18" t="s">
+      <c r="M19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="R19" s="14">
-        <v>1</v>
-      </c>
-      <c r="S19" s="16">
-        <v>1</v>
-      </c>
-      <c r="T19" s="16" t="s">
-        <v>68</v>
-      </c>
+      <c r="R19" s="12"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1290,18 +1176,12 @@
       <c r="L20" s="5">
         <v>4</v>
       </c>
-      <c r="M20" s="18" t="s">
+      <c r="M20" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="R20" s="14">
-        <v>2</v>
-      </c>
-      <c r="S20" s="16">
-        <v>2</v>
-      </c>
-      <c r="T20" s="16">
-        <v>1</v>
-      </c>
+      <c r="R20" s="12"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
     </row>
     <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -1331,15 +1211,9 @@
       <c r="I21" s="4">
         <v>5548731648</v>
       </c>
-      <c r="R21" s="14">
-        <v>3</v>
-      </c>
-      <c r="S21" s="16">
-        <v>2</v>
-      </c>
-      <c r="T21" s="16">
-        <v>2</v>
-      </c>
+      <c r="R21" s="12"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
     </row>
     <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1370,23 +1244,17 @@
         <v>5548731648</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L22" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22" s="9" t="s">
         <v>26</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R22" s="14">
-        <v>4</v>
-      </c>
-      <c r="S22" s="16">
-        <v>2</v>
-      </c>
-      <c r="T22" s="16">
-        <v>3</v>
-      </c>
+      <c r="R22" s="12"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
     </row>
     <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -1422,18 +1290,12 @@
       <c r="L23" s="5">
         <v>2</v>
       </c>
-      <c r="M23" s="18" t="s">
+      <c r="M23" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="R23" s="14">
-        <v>5</v>
-      </c>
-      <c r="S23" s="16">
-        <v>3</v>
-      </c>
-      <c r="T23" s="16">
-        <v>4</v>
-      </c>
+      <c r="R23" s="12"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
     </row>
     <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1469,18 +1331,12 @@
       <c r="L24" s="5">
         <v>2</v>
       </c>
-      <c r="M24" s="9" t="s">
+      <c r="M24" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="R24" s="14">
-        <v>6</v>
-      </c>
-      <c r="S24" s="16">
-        <v>3</v>
-      </c>
-      <c r="T24" s="16">
-        <v>5</v>
-      </c>
+      <c r="R24" s="12"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
     </row>
     <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -1516,18 +1372,12 @@
       <c r="L25" s="5">
         <v>2</v>
       </c>
-      <c r="M25" s="9" t="s">
+      <c r="M25" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="R25" s="14">
-        <v>7</v>
-      </c>
-      <c r="S25" s="16">
-        <v>4</v>
-      </c>
-      <c r="T25" s="16">
-        <v>6</v>
-      </c>
+      <c r="R25" s="12"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -1566,15 +1416,9 @@
       <c r="M26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="R26" s="14">
-        <v>8</v>
-      </c>
-      <c r="S26" s="16">
-        <v>4</v>
-      </c>
-      <c r="T26" s="16">
-        <v>7</v>
-      </c>
+      <c r="R26" s="12"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
     </row>
     <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -1610,9 +1454,12 @@
       <c r="L27" s="5">
         <v>3</v>
       </c>
-      <c r="M27" s="18" t="s">
+      <c r="M27" s="10" t="s">
         <v>42</v>
       </c>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
     </row>
     <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
@@ -1648,14 +1495,12 @@
       <c r="L28" s="5">
         <v>4</v>
       </c>
-      <c r="M28" s="18" t="s">
+      <c r="M28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="R28" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
     </row>
     <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
@@ -1694,15 +1539,9 @@
       <c r="M29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="R29" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="S29" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="T29" s="10" t="s">
-        <v>71</v>
-      </c>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
     </row>
     <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -1732,15 +1571,9 @@
       <c r="I30" s="4">
         <v>5548731648</v>
       </c>
-      <c r="R30">
-        <v>1</v>
-      </c>
-      <c r="S30">
-        <v>1</v>
-      </c>
-      <c r="T30">
-        <v>1</v>
-      </c>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -1773,21 +1606,15 @@
       <c r="K31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L31" s="11" t="s">
+      <c r="L31" s="9" t="s">
         <v>26</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R31">
-        <v>2</v>
-      </c>
-      <c r="S31">
-        <v>1</v>
-      </c>
-      <c r="T31">
-        <v>2</v>
-      </c>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
     </row>
     <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -1823,18 +1650,12 @@
       <c r="L32" s="6">
         <v>1</v>
       </c>
-      <c r="M32" s="9" t="s">
+      <c r="M32" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R32">
-        <v>3</v>
-      </c>
-      <c r="S32">
-        <v>2</v>
-      </c>
-      <c r="T32">
-        <v>3</v>
-      </c>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
     </row>
     <row r="33" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -1873,15 +1694,9 @@
       <c r="M33" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R33">
-        <v>4</v>
-      </c>
-      <c r="S33">
-        <v>2</v>
-      </c>
-      <c r="T33">
-        <v>4</v>
-      </c>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
     </row>
     <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -1920,15 +1735,9 @@
       <c r="M34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="R34">
-        <v>5</v>
-      </c>
-      <c r="S34">
-        <v>2</v>
-      </c>
-      <c r="T34">
-        <v>4</v>
-      </c>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
     </row>
     <row r="35" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1964,18 +1773,12 @@
       <c r="L35" s="6">
         <v>2</v>
       </c>
-      <c r="M35" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="R35">
-        <v>6</v>
-      </c>
-      <c r="S35">
-        <v>3</v>
-      </c>
-      <c r="T35">
-        <v>5</v>
-      </c>
+      <c r="M35" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
@@ -2011,18 +1814,12 @@
       <c r="L36" s="6">
         <v>2</v>
       </c>
-      <c r="M36" s="9" t="s">
+      <c r="M36" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="R36">
-        <v>7</v>
-      </c>
-      <c r="S36">
-        <v>4</v>
-      </c>
-      <c r="T36">
-        <v>4</v>
-      </c>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
     </row>
     <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
@@ -2061,15 +1858,9 @@
       <c r="M37" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R37">
-        <v>8</v>
-      </c>
-      <c r="S37">
-        <v>4</v>
-      </c>
-      <c r="T37">
-        <v>4</v>
-      </c>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
     </row>
     <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -2108,15 +1899,9 @@
       <c r="M38" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R38">
-        <v>9</v>
-      </c>
-      <c r="S38">
-        <v>4</v>
-      </c>
-      <c r="T38">
-        <v>4</v>
-      </c>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
@@ -2155,15 +1940,9 @@
       <c r="M39" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R39">
-        <v>10</v>
-      </c>
-      <c r="S39">
-        <v>4</v>
-      </c>
-      <c r="T39">
-        <v>4</v>
-      </c>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
     </row>
     <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
@@ -2202,15 +1981,9 @@
       <c r="M40" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R40">
-        <v>11</v>
-      </c>
-      <c r="S40">
-        <v>4</v>
-      </c>
-      <c r="T40">
-        <v>4</v>
-      </c>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
     </row>
     <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K41" s="5">

</xml_diff>